<commit_message>
added general changes to documentation
</commit_message>
<xml_diff>
--- a/data/Departamento_de_Justicia/djCasosMapa.xlsx
+++ b/data/Departamento_de_Justicia/djCasosMapa.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariana.pagan\Desktop\Comite PARE\Justicia\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/Estadisticas-Sobre-Violencia-de-Genero-en-Puerto-Rico/data/Departamento_de_Justicia/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6347F098-7EE8-4E46-85D2-2999277F8CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="10830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24280" windowHeight="10840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="djCasosMapa" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>Pueblo</t>
   </si>
@@ -505,15 +506,12 @@
   </si>
   <si>
     <t>cntyidfp</t>
-  </si>
-  <si>
-    <t>*Registro de Hombres Convictos por Violencia Doméstica. Datos acumulados desde el año 2018 hasta 27 de marzo de 2023.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1348,19 +1346,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1400,7 +1398,7 @@
         <v>-66.767099999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1420,7 +1418,7 @@
         <v>-67.1751</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1440,7 +1438,7 @@
         <v>-67.120800000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1458,7 @@
         <v>-66.126800000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1480,7 +1478,7 @@
         <v>-66.264099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1500,7 +1498,7 @@
         <v>-67.104399999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1520,7 +1518,7 @@
         <v>-66.675200000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1540,7 +1538,7 @@
         <v>-66.057400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1558,7 @@
         <v>-66.560500000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1578,7 @@
         <v>-66.309600000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1598,7 @@
         <v>-66.168400000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1620,7 +1618,7 @@
         <v>-67.156999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1640,7 +1638,7 @@
         <v>-66.050799999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1660,7 +1658,7 @@
         <v>-66.860200000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1680,7 +1678,7 @@
         <v>-65.883700000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1700,7 +1698,7 @@
         <v>-65.956800000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1720,7 +1718,7 @@
         <v>-66.143299999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>-66.160700000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1760,7 +1758,7 @@
         <v>-65.667699999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1780,7 +1778,7 @@
         <v>-66.516499999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1800,7 +1798,7 @@
         <v>-66.161199999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1820,7 +1818,7 @@
         <v>-66.363699999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1840,7 +1838,7 @@
         <v>-66.219899999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1860,7 +1858,7 @@
         <v>-66.330399999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1880,7 +1878,7 @@
         <v>-65.3095</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1900,7 +1898,7 @@
         <v>-66.278599999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1920,7 +1918,7 @@
         <v>-65.669799999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1938,7 @@
         <v>-66.560500000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1960,7 +1958,7 @@
         <v>-66.919700000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1980,7 +1978,7 @@
         <v>-66.135400000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -2000,7 +1998,7 @@
         <v>-66.793000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>-66.112200000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -2040,7 +2038,7 @@
         <v>-65.9786</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2060,7 +2058,7 @@
         <v>-66.796300000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>-67.114000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2100,7 +2098,7 @@
         <v>-65.810299999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -2120,7 +2118,7 @@
         <v>-67.005099999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2140,7 +2138,7 @@
         <v>-66.5916</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2160,7 +2158,7 @@
         <v>-66.493300000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -2180,7 +2178,7 @@
         <v>-65.909099999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2200,7 +2198,7 @@
         <v>-67.040700000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2220,7 +2218,7 @@
         <v>-66.8673</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2240,7 +2238,7 @@
         <v>-66.989900000000006</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2260,7 +2258,7 @@
         <v>-65.869500000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -2280,7 +2278,7 @@
         <v>-65.9114</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2300,7 +2298,7 @@
         <v>-65.725099999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2320,7 +2318,7 @@
         <v>-66.491</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2340,7 +2338,7 @@
         <v>-66.946299999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -2360,7 +2358,7 @@
         <v>-65.922200000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>-67.109499999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2400,7 +2398,7 @@
         <v>-67.0809</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -2420,7 +2418,7 @@
         <v>-66.415099999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -2440,7 +2438,7 @@
         <v>-65.770200000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -2460,7 +2458,7 @@
         <v>-66.252700000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -2480,7 +2478,7 @@
         <v>-66.433599999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -2500,7 +2498,7 @@
         <v>-66.012299999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -2520,7 +2518,7 @@
         <v>-66.721400000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -2540,7 +2538,7 @@
         <v>-66.6143</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -2560,7 +2558,7 @@
         <v>-66.926100000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -2580,7 +2578,7 @@
         <v>-67.231700000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>-65.813699999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>-66.943700000000007</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>-66.258099999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -2660,7 +2658,7 @@
         <v>-67.038600000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -2680,7 +2678,7 @@
         <v>-66.061099999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2700,7 +2698,7 @@
         <v>-65.976399999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2720,7 +2718,7 @@
         <v>-66.971199999999996</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -2740,7 +2738,7 @@
         <v>-66.388999999999996</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -2760,7 +2758,7 @@
         <v>-66.246600000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -2780,7 +2778,7 @@
         <v>-66.213999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -2800,7 +2798,7 @@
         <v>-65.998900000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -2820,7 +2818,7 @@
         <v>-66.703000000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -2840,7 +2838,7 @@
         <v>-66.337199999999996</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -2860,7 +2858,7 @@
         <v>-66.397900000000007</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -2880,7 +2878,7 @@
         <v>-65.453100000000006</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -2900,7 +2898,7 @@
         <v>-66.474800000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -2920,7 +2918,7 @@
         <v>-65.896299999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -2938,11 +2936,6 @@
       </c>
       <c r="F79">
         <v>-66.858800000000002</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>